<commit_message>
demo video si matrice testare
</commit_message>
<xml_diff>
--- a/Matrice_Testare.xlsx
+++ b/Matrice_Testare.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan\Desktop\facultate\POO\Calatoria-Cafelei-in-Romania\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037CDC1F-BA76-4272-BEC0-0EDEDDCD4247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
   <si>
     <t>ID Test</t>
   </si>
@@ -25,9 +31,6 @@
     <t>Scenariu de Testare</t>
   </si>
   <si>
-    <t>Pași</t>
-  </si>
-  <si>
     <t>Date de Intrare</t>
   </si>
   <si>
@@ -119,52 +122,6 @@
   </si>
   <si>
     <t>Ștergerea unui angajat existent de către Manager</t>
-  </si>
-  <si>
-    <t>1. Lansați aplicația.
-2. Introduceți username-ul și parola corecte.
-3. Apăsați Enter.</t>
-  </si>
-  <si>
-    <t>1. Lansați aplicația.
-2. Introduceți username-ul sau parola incorecte.
-3. Apăsați Enter.</t>
-  </si>
-  <si>
-    <t>1. Selectați opțiunea 'Sign up'.
-2. Introduceți informațiile necesare.
-3. Finalizați procesul.</t>
-  </si>
-  <si>
-    <t>1. Selectați un oraș din listă.</t>
-  </si>
-  <si>
-    <t>1. Introduceți o opțiune invalidă (e.g., 0 sau 6).</t>
-  </si>
-  <si>
-    <t>1. Autentificați-vă ca manager.
-2. Selectați opțiunea 'Adaugă angajat'.
-3. Completați informațiile angajatului.</t>
-  </si>
-  <si>
-    <t>1. Selectați opțiunea de generare raport.
-2. Alegeți limba română.
-3. Verificați fișierul 'raport.csv'.</t>
-  </si>
-  <si>
-    <t>1. Selectați opțiunea de generare raport.
-2. Alegeți limba engleză.
-3. Verificați fișierul 'raport.csv'.</t>
-  </si>
-  <si>
-    <t>1. Autentificați-vă.
-2. Selectați opțiunea 'Comandă'.
-3. Finalizați comanda.</t>
-  </si>
-  <si>
-    <t>1. Autentificați-vă ca manager.
-2. Selectați opțiunea 'Șterge angajat'.
-3. Alegeți angajatul dorit.</t>
   </si>
   <si>
     <t>Username: admin
@@ -229,13 +186,52 @@
   </si>
   <si>
     <t>Mesaj: 'Angajat șters cu succes!'</t>
+  </si>
+  <si>
+    <t>T011</t>
+  </si>
+  <si>
+    <t>Nume,Parola</t>
+  </si>
+  <si>
+    <t>Autentificare utilizator</t>
+  </si>
+  <si>
+    <t>Mesaj:'Autentificat cu succes!'</t>
+  </si>
+  <si>
+    <t>T012</t>
+  </si>
+  <si>
+    <t>Adaugare produse</t>
+  </si>
+  <si>
+    <t>Nume produs</t>
+  </si>
+  <si>
+    <t>Produs adaugat cu succes</t>
+  </si>
+  <si>
+    <t>passed</t>
+  </si>
+  <si>
+    <t>T013</t>
+  </si>
+  <si>
+    <t>Stergere produse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T014 </t>
+  </si>
+  <si>
+    <t>Adaugare eveniment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,12 +248,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -287,24 +289,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -342,7 +353,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -376,6 +387,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -410,9 +422,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -585,14 +598,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -602,220 +617,274 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>49</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
+        <v>50</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" t="s">
+        <v>51</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" t="s">
+        <v>52</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" t="s">
+        <v>53</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="F12" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="K12" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="B13" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="E13" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="F13" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="K13" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="B14" t="s">
         <v>64</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" t="s">
+        <v>66</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>